<commit_message>
State Machine: Added SM for aircraft simulation
</commit_message>
<xml_diff>
--- a/eVTOL_Simul_analysis.xlsx
+++ b/eVTOL_Simul_analysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/93045f396faa5efe/Desktop/Study_Material/Intership_prep/Joby/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/93045f396faa5efe/Desktop/Study_Material/Intership_prep/Joby/eVtol_simulation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="8_{9D6709F9-47CA-45E2-B41C-3BC805FFFB3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2615612D-A31C-433E-86C0-F576EA54D1B2}"/>
+  <xr:revisionPtr revIDLastSave="148" documentId="8_{9D6709F9-47CA-45E2-B41C-3BC805FFFB3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50A4579B-06D0-4AA3-B3B2-8EA9172AC311}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FD1416B5-478E-4032-BDC9-B3D0B3522E10}"/>
+    <workbookView xWindow="-19320" yWindow="135" windowWidth="19440" windowHeight="15600" xr2:uid="{FD1416B5-478E-4032-BDC9-B3D0B3522E10}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Company Name</t>
   </si>
@@ -59,19 +59,61 @@
     <t>Cruise Speed (mph)</t>
   </si>
   <si>
-    <t>Battery Capacity (kWh)</t>
-  </si>
-  <si>
-    <t>Time to Charge (hours)</t>
-  </si>
-  <si>
-    <t>Energy use at Cruise (kWh/mile)</t>
-  </si>
-  <si>
     <t>Passenger Count</t>
   </si>
   <si>
     <t>Probability of fault per hour</t>
+  </si>
+  <si>
+    <t>Stats</t>
+  </si>
+  <si>
+    <t>Physical world</t>
+  </si>
+  <si>
+    <t>Simulation world</t>
+  </si>
+  <si>
+    <t>hr</t>
+  </si>
+  <si>
+    <t>msec</t>
+  </si>
+  <si>
+    <t>Factor</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>battery threashold (%)</t>
+  </si>
+  <si>
+    <t>Battery Capacity (Wh)</t>
+  </si>
+  <si>
+    <t>Time to Charge (hours x 100)</t>
+  </si>
+  <si>
+    <t>Energy use at Cruise (Wh/mile)</t>
+  </si>
+  <si>
+    <t>Energy use per hour of flight (Wh/h)</t>
+  </si>
+  <si>
+    <t>Energy used per simulation time unit (Wh/t)</t>
+  </si>
+  <si>
+    <t>Battery capacity per % soc</t>
+  </si>
+  <si>
+    <t>Useable Battery capacity (Wh)</t>
+  </si>
+  <si>
+    <t>Downtime (h)</t>
+  </si>
+  <si>
+    <t>Miles travelled per simulation time unit (mile x 100)</t>
   </si>
 </sst>
 </file>
@@ -87,15 +129,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -103,12 +157,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -124,6 +196,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -443,163 +519,362 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68D37C5C-A2ED-4F78-B843-45B0592AC1E9}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.85546875" customWidth="1"/>
+    <col min="13" max="13" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>120</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>100</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>160</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>90</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="2">
+        <v>320000</v>
+      </c>
+      <c r="C3" s="2">
+        <v>100000</v>
+      </c>
+      <c r="D3" s="2">
+        <v>220000</v>
+      </c>
+      <c r="E3" s="2">
+        <v>120000</v>
+      </c>
+      <c r="F3" s="2">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2">
+        <v>60</v>
+      </c>
+      <c r="C4" s="2">
+        <v>20</v>
+      </c>
+      <c r="D4" s="2">
+        <v>80</v>
+      </c>
+      <c r="E4" s="2">
+        <v>62</v>
+      </c>
+      <c r="F4" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1600</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1500</v>
+      </c>
+      <c r="D5" s="2">
+        <v>2200</v>
+      </c>
+      <c r="E5" s="2">
+        <v>800</v>
+      </c>
+      <c r="F5" s="2">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
-        <v>320</v>
-      </c>
-      <c r="C3">
-        <v>100</v>
-      </c>
-      <c r="D3">
-        <v>220</v>
-      </c>
-      <c r="E3">
-        <v>120</v>
-      </c>
-      <c r="F3">
+      <c r="B6" s="2">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2">
+        <v>3</v>
+      </c>
+      <c r="E6" s="2">
+        <v>2</v>
+      </c>
+      <c r="F6" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="2">
+        <f>B3*(1-$O18)</f>
+        <v>288000</v>
+      </c>
+      <c r="C8" s="2">
+        <f t="shared" ref="C8:F8" si="0">C3*(1-$O18)</f>
+        <v>90000</v>
+      </c>
+      <c r="D8" s="2">
+        <f t="shared" si="0"/>
+        <v>198000</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="0"/>
+        <v>108000</v>
+      </c>
+      <c r="F8" s="2">
+        <f t="shared" si="0"/>
+        <v>135000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="2">
+        <f>B5*B2</f>
+        <v>192000</v>
+      </c>
+      <c r="C9" s="2">
+        <f t="shared" ref="C9:F9" si="1">C5*C2</f>
+        <v>150000</v>
+      </c>
+      <c r="D9" s="2">
+        <f t="shared" si="1"/>
+        <v>352000</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" si="1"/>
+        <v>72000</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="1"/>
+        <v>174000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="2">
+        <f>B9*$O17</f>
+        <v>192</v>
+      </c>
+      <c r="C10" s="2">
+        <f t="shared" ref="C10:F10" si="2">C9*$O17</f>
         <v>150</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4">
-        <v>0.6</v>
-      </c>
-      <c r="C4">
-        <v>0.2</v>
-      </c>
-      <c r="D4">
-        <v>0.8</v>
-      </c>
-      <c r="E4">
-        <v>0.62</v>
-      </c>
-      <c r="F4">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="D10" s="2">
+        <f t="shared" si="2"/>
+        <v>352</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" si="2"/>
+        <v>72</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" si="2"/>
+        <v>174</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="2">
+        <f>B3/100</f>
+        <v>3200</v>
+      </c>
+      <c r="C11" s="2">
+        <f t="shared" ref="C11:F11" si="3">C3/100</f>
+        <v>1000</v>
+      </c>
+      <c r="D11" s="2">
+        <f t="shared" si="3"/>
+        <v>2200</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="3"/>
+        <v>1200</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" si="3"/>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="2">
+        <f>100*B2*$O17</f>
+        <v>12</v>
+      </c>
+      <c r="C13" s="2">
+        <f t="shared" ref="C13:F13" si="4">100*C2*$O17</f>
+        <v>10</v>
+      </c>
+      <c r="D13" s="2">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="E13" s="2">
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="B5">
-        <v>1.6</v>
-      </c>
-      <c r="C5">
-        <v>1.5</v>
-      </c>
-      <c r="D5">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E5">
-        <v>0.8</v>
-      </c>
-      <c r="F5">
-        <v>5.8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="F13" s="2">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K16" t="s">
         <v>10</v>
       </c>
-      <c r="B6">
-        <v>4</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-      <c r="D6">
-        <v>3</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="F6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="M16" t="s">
         <v>11</v>
       </c>
-      <c r="B7">
-        <v>0.25</v>
-      </c>
-      <c r="C7">
+      <c r="O16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="10:15" x14ac:dyDescent="0.25">
+      <c r="J17" t="s">
+        <v>15</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17" t="s">
+        <v>12</v>
+      </c>
+      <c r="M17">
+        <v>1000</v>
+      </c>
+      <c r="N17" t="s">
+        <v>13</v>
+      </c>
+      <c r="O17">
+        <f>K17/M17</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="10:15" x14ac:dyDescent="0.25">
+      <c r="J18" t="s">
+        <v>16</v>
+      </c>
+      <c r="K18">
+        <v>10</v>
+      </c>
+      <c r="O18">
+        <f>K18/100</f>
         <v>0.1</v>
-      </c>
-      <c r="D7">
-        <v>0.05</v>
-      </c>
-      <c r="E7">
-        <v>0.22</v>
-      </c>
-      <c r="F7">
-        <v>0.61</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
State Machine: Updated the time scale for simulation
</commit_message>
<xml_diff>
--- a/eVTOL_Simul_analysis.xlsx
+++ b/eVTOL_Simul_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/93045f396faa5efe/Desktop/Study_Material/Intership_prep/Joby/eVtol_simulation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="148" documentId="8_{9D6709F9-47CA-45E2-B41C-3BC805FFFB3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50A4579B-06D0-4AA3-B3B2-8EA9172AC311}"/>
+  <xr:revisionPtr revIDLastSave="154" documentId="8_{9D6709F9-47CA-45E2-B41C-3BC805FFFB3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7EBD12D1-2F39-44A0-A303-9737BFB1E5A4}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="135" windowWidth="19440" windowHeight="15600" xr2:uid="{FD1416B5-478E-4032-BDC9-B3D0B3522E10}"/>
   </bookViews>
@@ -120,6 +120,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00000000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -176,11 +179,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -522,7 +526,7 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,6 +541,7 @@
     <col min="11" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.85546875" customWidth="1"/>
     <col min="13" max="13" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -735,23 +740,23 @@
       </c>
       <c r="B10" s="2">
         <f>B9*$O17</f>
-        <v>192</v>
+        <v>3.2</v>
       </c>
       <c r="C10" s="2">
         <f t="shared" ref="C10:F10" si="2">C9*$O17</f>
-        <v>150</v>
+        <v>2.5</v>
       </c>
       <c r="D10" s="2">
         <f t="shared" si="2"/>
-        <v>352</v>
+        <v>5.8666666666666671</v>
       </c>
       <c r="E10" s="2">
         <f t="shared" si="2"/>
-        <v>72</v>
+        <v>1.2</v>
       </c>
       <c r="F10" s="2">
         <f t="shared" si="2"/>
-        <v>174</v>
+        <v>2.9000000000000004</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -804,24 +809,24 @@
         <v>25</v>
       </c>
       <c r="B13" s="2">
-        <f>100*B2*$O17</f>
-        <v>12</v>
+        <f>10000*B2*$O17</f>
+        <v>20</v>
       </c>
       <c r="C13" s="2">
-        <f t="shared" ref="C13:F13" si="4">100*C2*$O17</f>
-        <v>10</v>
+        <f t="shared" ref="C13:F13" si="4">10000*C2*$O17</f>
+        <v>16.666666666666668</v>
       </c>
       <c r="D13" s="2">
         <f t="shared" si="4"/>
-        <v>16</v>
+        <v>26.666666666666668</v>
       </c>
       <c r="E13" s="2">
         <f t="shared" si="4"/>
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F13" s="2">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -851,14 +856,14 @@
         <v>12</v>
       </c>
       <c r="M17">
-        <v>1000</v>
+        <v>60000</v>
       </c>
       <c r="N17" t="s">
         <v>13</v>
       </c>
-      <c r="O17">
+      <c r="O17" s="4">
         <f>K17/M17</f>
-        <v>1E-3</v>
+        <v>1.6666666666666667E-5</v>
       </c>
     </row>
     <row r="18" spans="10:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Simulation: Fixed data types for logging parameters. Tested all services
</commit_message>
<xml_diff>
--- a/eVTOL_Simul_analysis.xlsx
+++ b/eVTOL_Simul_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/93045f396faa5efe/Desktop/Study_Material/Intership_prep/Joby/eVtol_simulation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="154" documentId="8_{9D6709F9-47CA-45E2-B41C-3BC805FFFB3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7EBD12D1-2F39-44A0-A303-9737BFB1E5A4}"/>
+  <xr:revisionPtr revIDLastSave="174" documentId="8_{9D6709F9-47CA-45E2-B41C-3BC805FFFB3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86A9ECE9-AB74-4946-B98F-6085C7C44AC5}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="135" windowWidth="19440" windowHeight="15600" xr2:uid="{FD1416B5-478E-4032-BDC9-B3D0B3522E10}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Company Name</t>
   </si>
@@ -113,7 +113,16 @@
     <t>Downtime (h)</t>
   </si>
   <si>
-    <t>Miles travelled per simulation time unit (mile x 100)</t>
+    <t>Miles travelled per simulation time unit (mile)</t>
+  </si>
+  <si>
+    <t>Analysis</t>
+  </si>
+  <si>
+    <t>Filght time in one charge (hr)</t>
+  </si>
+  <si>
+    <t>Miles travelled in one charge (mile)</t>
   </si>
 </sst>
 </file>
@@ -179,12 +188,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,7 +536,7 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -809,32 +819,58 @@
         <v>25</v>
       </c>
       <c r="B13" s="2">
-        <f>10000*B2*$O17</f>
-        <v>20</v>
+        <f>B2*$O17</f>
+        <v>2E-3</v>
       </c>
       <c r="C13" s="2">
-        <f t="shared" ref="C13:F13" si="4">10000*C2*$O17</f>
-        <v>16.666666666666668</v>
+        <f t="shared" ref="C13:F13" si="4">C2*$O17</f>
+        <v>1.6666666666666668E-3</v>
       </c>
       <c r="D13" s="2">
         <f t="shared" si="4"/>
-        <v>26.666666666666668</v>
+        <v>2.666666666666667E-3</v>
       </c>
       <c r="E13" s="2">
         <f t="shared" si="4"/>
-        <v>15</v>
+        <v>1.5E-3</v>
       </c>
       <c r="F13" s="2">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>5.0000000000000001E-4</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="K15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16">
+        <f>B17/B2</f>
+        <v>1.5</v>
+      </c>
+      <c r="C16">
+        <f t="shared" ref="C16:F16" si="5">C17/C2</f>
+        <v>0.6</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="5"/>
+        <v>0.5625</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="5"/>
+        <v>1.5</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="5"/>
+        <v>0.77586206896551724</v>
+      </c>
       <c r="K16" t="s">
         <v>10</v>
       </c>
@@ -845,7 +881,30 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="10:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17">
+        <f>B8/B5</f>
+        <v>180</v>
+      </c>
+      <c r="C17">
+        <f t="shared" ref="C17:F17" si="6">C8/C5</f>
+        <v>60</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="6"/>
+        <v>90</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="6"/>
+        <v>135</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="6"/>
+        <v>23.275862068965516</v>
+      </c>
       <c r="J17" t="s">
         <v>15</v>
       </c>
@@ -866,7 +925,7 @@
         <v>1.6666666666666667E-5</v>
       </c>
     </row>
-    <row r="18" spans="10:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J18" t="s">
         <v>16</v>
       </c>

</xml_diff>